<commit_message>
Añadiendo binario mas capas
</commit_message>
<xml_diff>
--- a/CuadroResultadosModelo.xlsx
+++ b/CuadroResultadosModelo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel\Desktop\dockerfiles\aprendizaje_profundo\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanes08/Documents/Maestria/2_Semestre/AprendizajeProfundo/proyecto/repo/Aprendizaje_profundo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AA0D9CD-FFD8-49D0-8610-B4685BD6FBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C405351B-4184-D747-9B30-9DDC878E805D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-38400" yWindow="-12680" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="78">
   <si>
     <t>Detección automática de cubrebocas a través de redes convolucionales</t>
   </si>
@@ -333,11 +333,41 @@
     <t>Train: 0.9934
 Test: 0.9502</t>
   </si>
+  <si>
+    <t>64 X 64 X 1
+64 X 64 X 16
+32 X 32 X 16
+32 X 32 X 32
+16 X 16 X 32
+16 X 16 X 64
+8 X 8 X 64
+4,096
+256
+128
+64
+2</t>
+  </si>
+  <si>
+    <t>Train: 0.2033
+Test: 0.2071</t>
+  </si>
+  <si>
+    <t>Train: 0.9708
+Test:0.9609</t>
+  </si>
+  <si>
+    <t>Precision:
+Train: 0.96
+Test: 0.95
+Recall:
+Train: 0.93
+Test: 0.95</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20">
     <font>
       <sz val="11"/>
@@ -619,25 +649,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="Accent" xfId="2"/>
-    <cellStyle name="Accent 1" xfId="3"/>
-    <cellStyle name="Accent 2" xfId="4"/>
-    <cellStyle name="Accent 3" xfId="5"/>
-    <cellStyle name="Bad" xfId="6"/>
-    <cellStyle name="Error" xfId="7"/>
-    <cellStyle name="Footnote" xfId="8"/>
-    <cellStyle name="Good" xfId="9"/>
-    <cellStyle name="Heading" xfId="10"/>
-    <cellStyle name="Heading 1" xfId="11"/>
-    <cellStyle name="Heading 2" xfId="12"/>
-    <cellStyle name="Hyperlink" xfId="13"/>
+    <cellStyle name="Accent" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Bad" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Error" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Footnote" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Good" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Heading" xfId="10" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Heading 1" xfId="11" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Heading 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Hyperlink" xfId="13" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Note" xfId="14"/>
-    <cellStyle name="Result" xfId="15"/>
-    <cellStyle name="Status" xfId="16"/>
-    <cellStyle name="Text" xfId="17"/>
-    <cellStyle name="Warning" xfId="18"/>
+    <cellStyle name="Note" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Result" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Status" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Text" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Warning" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -948,28 +978,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="3" width="51.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="51.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
     <col min="10" max="11" width="16.6640625" customWidth="1"/>
     <col min="12" max="12" width="21.33203125" customWidth="1"/>
-    <col min="13" max="26" width="13.88671875" customWidth="1"/>
-    <col min="27" max="64" width="18.77734375" customWidth="1"/>
+    <col min="13" max="26" width="13.83203125" customWidth="1"/>
+    <col min="27" max="64" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="14.25" customHeight="1"/>
@@ -1037,7 +1067,7 @@
       </c>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="2:13" ht="172.8">
+    <row r="9" spans="2:13" ht="192">
       <c r="B9" s="6" t="s">
         <v>17</v>
       </c>
@@ -1159,7 +1189,7 @@
       <c r="L14" s="6"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="2:13" ht="14.4">
+    <row r="15" spans="2:13">
       <c r="B15" s="6" t="s">
         <v>17</v>
       </c>
@@ -1267,7 +1297,7 @@
       <c r="L20" s="6"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="2:13" ht="100.8">
+    <row r="21" spans="2:13" ht="112">
       <c r="B21" s="6" t="s">
         <v>17</v>
       </c>
@@ -1301,7 +1331,7 @@
       <c r="L21" s="8"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="2:13" ht="100.8">
+    <row r="22" spans="2:13" ht="112">
       <c r="B22" s="6" t="s">
         <v>17</v>
       </c>
@@ -1335,7 +1365,7 @@
       <c r="L22" s="6"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="2:13" ht="158.4">
+    <row r="23" spans="2:13" ht="176">
       <c r="B23" s="6" t="s">
         <v>17</v>
       </c>
@@ -1367,7 +1397,7 @@
       <c r="L23" s="6"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="2:13" ht="14.4">
+    <row r="24" spans="2:13">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="7"/>
@@ -1381,7 +1411,7 @@
       <c r="L24" s="6"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="2:13" ht="259.2">
+    <row r="25" spans="2:13" ht="288">
       <c r="B25" s="6" t="s">
         <v>17</v>
       </c>
@@ -1665,7 +1695,7 @@
       <c r="L39" s="6"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="2:13" ht="172.8">
+    <row r="40" spans="2:13" ht="192">
       <c r="B40" s="6" t="s">
         <v>38</v>
       </c>
@@ -1881,7 +1911,7 @@
       <c r="L50" s="6"/>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="2:13" ht="14.25" customHeight="1">
+    <row r="51" spans="2:13" ht="14" customHeight="1">
       <c r="B51" s="6" t="s">
         <v>38</v>
       </c>
@@ -1899,22 +1929,38 @@
       <c r="L51" s="6"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="2:13" ht="14.25" customHeight="1">
+    <row r="52" spans="2:13" ht="216" customHeight="1">
       <c r="B52" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
+      <c r="D52" s="7">
+        <v>1103090</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
+      <c r="L52" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="M52" s="3"/>
     </row>
     <row r="53" spans="2:13" ht="14.25" customHeight="1">
@@ -3199,18 +3245,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.109375" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" customWidth="1"/>
+    <col min="1" max="1" width="41.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
     <col min="3" max="3" width="48.6640625" customWidth="1"/>
-    <col min="4" max="26" width="13.88671875" customWidth="1"/>
-    <col min="27" max="64" width="18.77734375" customWidth="1"/>
+    <col min="4" max="26" width="13.83203125" customWidth="1"/>
+    <col min="27" max="64" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
modelo sin regularizacion de dos salidas
</commit_message>
<xml_diff>
--- a/CuadroResultadosModelo.xlsx
+++ b/CuadroResultadosModelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA287D5-BC84-41B7-837D-76372CCFF525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44353449-6C9D-46C2-B6A3-EC7673EC484D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="85">
   <si>
     <t>Detección automática de cubrebocas a través de redes convolucionales</t>
   </si>
@@ -382,12 +382,20 @@
     <t>Train:0.9917
 Test: 0.9532</t>
   </si>
+  <si>
+    <t>Train: 0.0427
+Test:0.0570</t>
+  </si>
+  <si>
+    <t>Train:0.9937
+Test: 0.9746</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -518,6 +526,12 @@
       <color rgb="FF000000"/>
       <name val="Var(--jp-code-font-family)"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF212121"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -638,7 +652,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -675,6 +689,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1009,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M1048571"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1785,22 +1800,34 @@
       <c r="L40" s="6"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="2:13" ht="14.25" customHeight="1">
+    <row r="41" spans="2:13" ht="172.8">
       <c r="B41" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="8"/>
+      <c r="D41" s="7">
+        <v>1103025</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
+      <c r="G41" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H41" s="16">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
       <c r="M41" s="3"/>
     </row>
     <row r="42" spans="2:13" ht="14.25" customHeight="1">

</xml_diff>